<commit_message>
handle initial matrix export independent of algorithm condition
</commit_message>
<xml_diff>
--- a/AIDA_basic/Results/DSM_Permutated_LA.xlsx
+++ b/AIDA_basic/Results/DSM_Permutated_LA.xlsx
@@ -492,92 +492,92 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
+          <t>Manage Mission Modes</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Sense and Avoid Obstacles</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Build FlightPlan Relative to Aircraft Type</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>CheckWinfForce</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Retrieve POI</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Identify Absolute Aircraft Coordinates</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Identify Defects</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Send Pictures to DB</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Generate Thrust</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Monitor UAV Control</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Manage Photos Recording</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>Record photos and videos</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>Control Camera Orientation</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>Configurate Flight Plan</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>Send moving obstacle position</t>
+        </is>
+      </c>
+      <c r="R1" s="2" t="inlineStr">
+        <is>
+          <t>Send stationary obstacle position</t>
+        </is>
+      </c>
+      <c r="S1" s="2" t="inlineStr">
+        <is>
+          <t>Send/Receive data</t>
+        </is>
+      </c>
+      <c r="T1" s="2" t="inlineStr">
+        <is>
           <t>Emergency Landing</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Identify Defects</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Retrieve POI</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Manage Mission Modes</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Generate Thrust</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Build FlightPlan Relative to Aircraft Type</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>Monitor UAV Control</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>Manage Photos Recording</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>Identify Absolute Aircraft Coordinates</t>
-        </is>
-      </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Sense and Avoid Obstacles</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>Send Pictures to DB</t>
-        </is>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>CheckWinfForce</t>
-        </is>
-      </c>
-      <c r="O1" s="2" t="inlineStr">
-        <is>
-          <t>Control Camera Orientation</t>
-        </is>
-      </c>
-      <c r="P1" s="2" t="inlineStr">
-        <is>
-          <t>Record photos and videos</t>
-        </is>
-      </c>
-      <c r="Q1" s="2" t="inlineStr">
-        <is>
-          <t>Configurate Flight Plan</t>
-        </is>
-      </c>
-      <c r="R1" s="2" t="inlineStr">
-        <is>
-          <t>Send moving obstacle position</t>
-        </is>
-      </c>
-      <c r="S1" s="2" t="inlineStr">
-        <is>
-          <t>Send stationary obstacle position</t>
-        </is>
-      </c>
-      <c r="T1" s="2" t="inlineStr">
-        <is>
-          <t>Send/Receive data</t>
         </is>
       </c>
       <c r="U1" s="2" t="inlineStr">
@@ -646,13 +646,13 @@
         <v>0</v>
       </c>
       <c r="N2" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="P2" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="5" t="n">
         <v>0</v>
@@ -682,7 +682,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Emergency Landing</t>
+          <t>Manage Mission Modes</t>
         </is>
       </c>
       <c r="B3" s="5" t="n">
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>0</v>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="5" t="n">
         <v>0</v>
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="5" t="n">
         <v>0</v>
@@ -760,7 +760,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Identify Defects</t>
+          <t>Sense and Avoid Obstacles</t>
         </is>
       </c>
       <c r="B4" s="5" t="n">
@@ -823,10 +823,10 @@
         <v>0</v>
       </c>
       <c r="U4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="5" t="n">
         <v>0</v>
@@ -838,7 +838,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Retrieve POI</t>
+          <t>Build FlightPlan Relative to Aircraft Type</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
@@ -848,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>0</v>
@@ -901,10 +901,10 @@
         <v>0</v>
       </c>
       <c r="U5" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" s="5" t="n">
         <v>0</v>
@@ -916,7 +916,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Manage Mission Modes</t>
+          <t>CheckWinfForce</t>
         </is>
       </c>
       <c r="B6" s="5" t="n">
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
@@ -946,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>0</v>
@@ -994,7 +994,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Generate Thrust</t>
+          <t>Retrieve POI</t>
         </is>
       </c>
       <c r="B7" s="5" t="n">
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="5" t="n">
         <v>0</v>
@@ -1057,22 +1057,22 @@
         <v>0</v>
       </c>
       <c r="U7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="X7" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Build FlightPlan Relative to Aircraft Type</t>
+          <t>Identify Absolute Aircraft Coordinates</t>
         </is>
       </c>
       <c r="B8" s="5" t="n">
@@ -1085,13 +1085,13 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="4" t="inlineStr">
         <is>
@@ -1150,7 +1150,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Monitor UAV Control</t>
+          <t>Identify Defects</t>
         </is>
       </c>
       <c r="B9" s="5" t="n">
@@ -1222,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="X9" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Manage Photos Recording</t>
+          <t>Send Pictures to DB</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
@@ -1253,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="4" t="inlineStr">
         <is>
@@ -1267,16 +1267,16 @@
         <v>0</v>
       </c>
       <c r="M10" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="O10" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="5" t="n">
         <v>0</v>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" s="5" t="n">
         <v>0</v>
@@ -1306,7 +1306,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Identify Absolute Aircraft Coordinates</t>
+          <t>Generate Thrust</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5" t="n">
         <v>0</v>
@@ -1378,13 +1378,13 @@
         <v>0</v>
       </c>
       <c r="X11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Sense and Avoid Obstacles</t>
+          <t>Monitor UAV Control</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">
@@ -1447,22 +1447,22 @@
         <v>0</v>
       </c>
       <c r="U12" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="X12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Send Pictures to DB</t>
+          <t>Manage Photos Recording</t>
         </is>
       </c>
       <c r="B13" s="5" t="n">
@@ -1472,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>0</v>
@@ -1490,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>0</v>
@@ -1504,10 +1504,10 @@
         </is>
       </c>
       <c r="N13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="5" t="n">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="5" t="n">
         <v>0</v>
@@ -1540,7 +1540,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>CheckWinfForce</t>
+          <t>Record photos and videos</t>
         </is>
       </c>
       <c r="B14" s="5" t="n">
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
@@ -1585,7 +1585,7 @@
         </is>
       </c>
       <c r="O14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="5" t="n">
         <v>0</v>
@@ -1696,7 +1696,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Record photos and videos</t>
+          <t>Configurate Flight Plan</t>
         </is>
       </c>
       <c r="B16" s="5" t="n">
@@ -1709,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5" t="n">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="4" t="inlineStr">
         <is>
@@ -1774,7 +1774,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Configurate Flight Plan</t>
+          <t>Send moving obstacle position</t>
         </is>
       </c>
       <c r="B17" s="5" t="n">
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>0</v>
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="5" t="n">
         <v>0</v>
@@ -1852,7 +1852,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Send moving obstacle position</t>
+          <t>Send stationary obstacle position</t>
         </is>
       </c>
       <c r="B18" s="5" t="n">
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="5" t="n">
         <v>0</v>
@@ -1930,7 +1930,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>Send stationary obstacle position</t>
+          <t>Send/Receive data</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5" t="n">
         <v>0</v>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="5" t="n">
         <v>0</v>
@@ -2008,7 +2008,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Send/Receive data</t>
+          <t>Emergency Landing</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
@@ -2030,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="5" t="n">
         <v>0</v>
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="5" t="n">
         <v>0</v>
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="5" t="n">
         <v>0</v>
@@ -2183,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="5" t="n">
         <v>0</v>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="5" t="n">
         <v>0</v>
@@ -2258,31 +2258,31 @@
         <v>0</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="N23" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="5" t="n">
         <v>0</v>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>0</v>
@@ -2336,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="5" t="n">
         <v>0</v>
@@ -2428,42 +2428,42 @@
       </c>
       <c r="G25" s="5" t="inlineStr">
         <is>
+          <t>Mission Mgt Subsystem</t>
+        </is>
+      </c>
+      <c r="H25" s="5" t="inlineStr">
+        <is>
+          <t>Mission Mgt Subsystem</t>
+        </is>
+      </c>
+      <c r="I25" s="5" t="inlineStr">
+        <is>
+          <t>Mission Mgt Subsystem</t>
+        </is>
+      </c>
+      <c r="J25" s="5" t="inlineStr">
+        <is>
+          <t>Mission Mgt Subsystem</t>
+        </is>
+      </c>
+      <c r="K25" s="5" t="inlineStr">
+        <is>
           <t>Propulsion Subsystem</t>
         </is>
       </c>
-      <c r="H25" s="5" t="inlineStr">
+      <c r="L25" s="5" t="inlineStr">
         <is>
           <t>UAV Control Station Subsystem</t>
         </is>
       </c>
-      <c r="I25" s="5" t="inlineStr">
-        <is>
-          <t>UAV Control Station Subsystem</t>
-        </is>
-      </c>
-      <c r="J25" s="5" t="inlineStr">
-        <is>
-          <t>UAV Control Station Subsystem</t>
-        </is>
-      </c>
-      <c r="K25" s="5" t="inlineStr">
-        <is>
-          <t>UAV Control Station Subsystem</t>
-        </is>
-      </c>
-      <c r="L25" s="5" t="inlineStr">
-        <is>
-          <t>UAV Control Station Subsystem</t>
-        </is>
-      </c>
       <c r="M25" s="5" t="inlineStr">
         <is>
-          <t>UAV Control Station Subsystem</t>
+          <t>Vision Subsystem</t>
         </is>
       </c>
       <c r="N25" s="5" t="inlineStr">
         <is>
-          <t>UAV Control Station Subsystem</t>
+          <t>Vision Subsystem</t>
         </is>
       </c>
       <c r="O25" s="5" t="inlineStr">
@@ -2473,27 +2473,27 @@
       </c>
       <c r="P25" s="5" t="inlineStr">
         <is>
-          <t>Vision Subsystem</t>
+          <t>Airline Human Operator</t>
         </is>
       </c>
       <c r="Q25" s="5" t="inlineStr">
         <is>
-          <t>Airline Human Operator</t>
+          <t>Moving Obstacles</t>
         </is>
       </c>
       <c r="R25" s="5" t="inlineStr">
         <is>
-          <t>Moving Obstacles</t>
+          <t>Stationary Obstacle</t>
         </is>
       </c>
       <c r="S25" s="5" t="inlineStr">
         <is>
-          <t>Stationary Obstacle</t>
+          <t>Aircraft Company Database</t>
         </is>
       </c>
       <c r="T25" s="5" t="inlineStr">
         <is>
-          <t>Aircraft Company Database</t>
+          <t>Flight Mgt Subsystem</t>
         </is>
       </c>
       <c r="U25" s="5" t="inlineStr">

</xml_diff>

<commit_message>
dsm matrix permutated styled
</commit_message>
<xml_diff>
--- a/AIDA_basic/Results/DSM_Permutated_LA.xlsx
+++ b/AIDA_basic/Results/DSM_Permutated_LA.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -38,12 +38,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00070C13"/>
-        <bgColor rgb="00070C13"/>
+        <fgColor rgb="00EBF1DE"/>
+        <bgColor rgb="00EBF1DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C5D9F1"/>
+        <bgColor rgb="00C5D9F1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,31 +63,28 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -449,38 +452,38 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="44" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="20" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
-    <col width="20" customWidth="1" min="21" max="21"/>
-    <col width="20" customWidth="1" min="22" max="22"/>
-    <col width="20" customWidth="1" min="23" max="23"/>
-    <col width="20" customWidth="1" min="24" max="24"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -693,25 +696,25 @@
           <t>F2</t>
         </is>
       </c>
-      <c r="D3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5" t="n">
+      <c r="D3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="5" t="n">
@@ -766,7 +769,7 @@
       <c r="B4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -774,22 +777,22 @@
           <t>F3</t>
         </is>
       </c>
-      <c r="E4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5" t="n">
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K4" s="5" t="n">
@@ -844,10 +847,10 @@
       <c r="B5" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="n">
+      <c r="C5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -855,19 +858,19 @@
           <t>F4</t>
         </is>
       </c>
-      <c r="F5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5" t="n">
+      <c r="F5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="5" t="n">
@@ -922,13 +925,13 @@
       <c r="B6" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="n">
+      <c r="C6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="inlineStr">
@@ -936,16 +939,16 @@
           <t>F5</t>
         </is>
       </c>
-      <c r="G6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5" t="n">
+      <c r="G6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="5" t="n">
@@ -1000,16 +1003,16 @@
       <c r="B7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5" t="n">
+      <c r="C7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -1017,13 +1020,13 @@
           <t>F6</t>
         </is>
       </c>
-      <c r="H7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5" t="n">
+      <c r="H7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="5" t="n">
@@ -1078,19 +1081,19 @@
       <c r="B8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5" t="n">
+      <c r="C8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="4" t="inlineStr">
@@ -1098,10 +1101,10 @@
           <t>F7</t>
         </is>
       </c>
-      <c r="I8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5" t="n">
+      <c r="I8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K8" s="5" t="n">
@@ -1156,22 +1159,22 @@
       <c r="B9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="n">
+      <c r="C9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="4" t="inlineStr">
@@ -1179,7 +1182,7 @@
           <t>F8</t>
         </is>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="4" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="5" t="n">
@@ -1234,25 +1237,25 @@
       <c r="B10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="n">
+      <c r="C10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4" t="n">
         <v>1</v>
       </c>
       <c r="J10" s="4" t="inlineStr">
@@ -1503,10 +1506,10 @@
           <t>F12</t>
         </is>
       </c>
-      <c r="N13" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="5" t="n">
+      <c r="N13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4" t="n">
         <v>1</v>
       </c>
       <c r="P13" s="5" t="n">
@@ -1576,7 +1579,7 @@
       <c r="L14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="M14" s="5" t="n">
+      <c r="M14" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N14" s="4" t="inlineStr">
@@ -1584,7 +1587,7 @@
           <t>F13</t>
         </is>
       </c>
-      <c r="O14" s="5" t="n">
+      <c r="O14" s="4" t="n">
         <v>1</v>
       </c>
       <c r="P14" s="5" t="n">
@@ -1654,10 +1657,10 @@
       <c r="L15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="M15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5" t="n">
+      <c r="M15" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O15" s="4" t="inlineStr">
@@ -2070,10 +2073,10 @@
           <t>F19</t>
         </is>
       </c>
-      <c r="U20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" s="5" t="n">
+      <c r="U20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="W20" s="5" t="n">
@@ -2143,7 +2146,7 @@
       <c r="S21" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="T21" s="5" t="n">
+      <c r="T21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="U21" s="4" t="inlineStr">
@@ -2151,7 +2154,7 @@
           <t>F20</t>
         </is>
       </c>
-      <c r="V21" s="5" t="n">
+      <c r="V21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="W21" s="5" t="n">
@@ -2221,10 +2224,10 @@
       <c r="S22" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="T22" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U22" s="5" t="n">
+      <c r="T22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="V22" s="4" t="inlineStr">
@@ -2396,122 +2399,122 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="inlineStr">
+      <c r="A25" s="6" t="inlineStr">
         <is>
           <t>LogicalComponentName</t>
         </is>
       </c>
-      <c r="B25" s="5" t="inlineStr">
+      <c r="B25" s="4" t="inlineStr">
         <is>
           <t>Aircraft</t>
         </is>
       </c>
-      <c r="C25" s="5" t="inlineStr">
+      <c r="C25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="D25" s="5" t="inlineStr">
+      <c r="D25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="E25" s="5" t="inlineStr">
+      <c r="E25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="F25" s="5" t="inlineStr">
+      <c r="F25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="G25" s="5" t="inlineStr">
+      <c r="G25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="H25" s="5" t="inlineStr">
+      <c r="H25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="I25" s="5" t="inlineStr">
+      <c r="I25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="J25" s="5" t="inlineStr">
+      <c r="J25" s="4" t="inlineStr">
         <is>
           <t>Mission Mgt Subsystem</t>
         </is>
       </c>
-      <c r="K25" s="5" t="inlineStr">
+      <c r="K25" s="4" t="inlineStr">
         <is>
           <t>Propulsion Subsystem</t>
         </is>
       </c>
-      <c r="L25" s="5" t="inlineStr">
+      <c r="L25" s="4" t="inlineStr">
         <is>
           <t>UAV Control Station Subsystem</t>
         </is>
       </c>
-      <c r="M25" s="5" t="inlineStr">
+      <c r="M25" s="4" t="inlineStr">
         <is>
           <t>Vision Subsystem</t>
         </is>
       </c>
-      <c r="N25" s="5" t="inlineStr">
+      <c r="N25" s="4" t="inlineStr">
         <is>
           <t>Vision Subsystem</t>
         </is>
       </c>
-      <c r="O25" s="5" t="inlineStr">
+      <c r="O25" s="4" t="inlineStr">
         <is>
           <t>Vision Subsystem</t>
         </is>
       </c>
-      <c r="P25" s="5" t="inlineStr">
+      <c r="P25" s="4" t="inlineStr">
         <is>
           <t>Airline Human Operator</t>
         </is>
       </c>
-      <c r="Q25" s="5" t="inlineStr">
+      <c r="Q25" s="4" t="inlineStr">
         <is>
           <t>Moving Obstacles</t>
         </is>
       </c>
-      <c r="R25" s="5" t="inlineStr">
+      <c r="R25" s="4" t="inlineStr">
         <is>
           <t>Stationary Obstacle</t>
         </is>
       </c>
-      <c r="S25" s="5" t="inlineStr">
+      <c r="S25" s="4" t="inlineStr">
         <is>
           <t>Aircraft Company Database</t>
         </is>
       </c>
-      <c r="T25" s="5" t="inlineStr">
+      <c r="T25" s="4" t="inlineStr">
         <is>
           <t>Flight Mgt Subsystem</t>
         </is>
       </c>
-      <c r="U25" s="5" t="inlineStr">
+      <c r="U25" s="4" t="inlineStr">
         <is>
           <t>Flight Mgt Subsystem</t>
         </is>
       </c>
-      <c r="V25" s="5" t="inlineStr">
+      <c r="V25" s="4" t="inlineStr">
         <is>
           <t>Flight Mgt Subsystem</t>
         </is>
       </c>
-      <c r="W25" s="5" t="inlineStr">
+      <c r="W25" s="4" t="inlineStr">
         <is>
           <t>Air/ Terrestrian Gravity</t>
         </is>
       </c>
-      <c r="X25" s="5" t="inlineStr">
+      <c r="X25" s="4" t="inlineStr">
         <is>
           <t>UAV Pilot</t>
         </is>

</xml_diff>